<commit_message>
Habilidades de enemigos y bosses
</commit_message>
<xml_diff>
--- a/Docs/Plantilla de habilidades.xlsx
+++ b/Docs/Plantilla de habilidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\Proyectos VS\Proyectazo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UTN\2022\Lab II\PROYECTAZO\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD55FA0F-3FED-42DA-9ADA-97CBB84287A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DE8668-0AD9-4312-A6FD-BFA8AA8943CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13230" yWindow="2805" windowWidth="15510" windowHeight="11190" xr2:uid="{F289420B-928D-4B6D-9A00-B13F97946B31}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F289420B-928D-4B6D-9A00-B13F97946B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,8 +629,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -679,6 +692,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -692,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -745,6 +764,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1342,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1575B6-EC1A-4D1D-8BD4-746F0EB28CFF}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,10 +1440,10 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1429,10 +1460,10 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -1446,10 +1477,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1466,10 +1497,10 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1489,10 +1520,10 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1517,10 +1548,10 @@
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1541,10 +1572,10 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1575,7 +1606,7 @@
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1602,7 +1633,7 @@
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1625,7 +1656,7 @@
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1651,7 +1682,7 @@
       <c r="A13" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1674,7 +1705,7 @@
       <c r="A14" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1700,7 +1731,7 @@
       <c r="A15" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1729,7 +1760,7 @@
       <c r="A16" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1758,7 +1789,7 @@
       <c r="A17" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -1781,7 +1812,7 @@
       <c r="A18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1804,7 +1835,7 @@
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -1827,7 +1858,7 @@
       <c r="A20" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1850,7 +1881,7 @@
       <c r="A21" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1873,7 +1904,7 @@
       <c r="A22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="20" t="s">
         <v>6</v>
       </c>
       <c r="D22" s="1" t="s">

</xml_diff>

<commit_message>
completadas casi todas las habilidades
</commit_message>
<xml_diff>
--- a/Docs/Plantilla de habilidades.xlsx
+++ b/Docs/Plantilla de habilidades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UTN\2022\Lab II\PROYECTAZO\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\Desktop\Proyectos VS\Proyectazo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555D40D5-538C-4C95-B64C-DEB23B41C3B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204AC2F0-D49C-4F4A-8CA4-C3D3A14A190E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F289420B-928D-4B6D-9A00-B13F97946B31}"/>
+    <workbookView xWindow="4695" yWindow="2865" windowWidth="21600" windowHeight="11385" xr2:uid="{F289420B-928D-4B6D-9A00-B13F97946B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Habilidades" sheetId="1" r:id="rId1"/>
@@ -366,9 +366,6 @@
     <t>Habilidades</t>
   </si>
   <si>
-    <t>10% de resistencia a todos los elementos y los ataques básicos hacen daño de tierra</t>
-  </si>
-  <si>
     <t>Columna1</t>
   </si>
   <si>
@@ -577,13 +574,16 @@
   </si>
   <si>
     <t>xp a subir</t>
+  </si>
+  <si>
+    <t>40% de defensa física y defensa mágica por 3 turnos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,13 +651,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -677,42 +670,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8181"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -723,12 +686,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,6 +707,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -763,7 +726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -771,69 +734,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1429,16 +1375,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C1575B6-EC1A-4D1D-8BD4-746F0EB28CFF}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F22" sqref="A22:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="57.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
@@ -1448,28 +1393,28 @@
   <sheetData>
     <row r="1" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1489,609 +1434,638 @@
         <v>67</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+    <row r="3" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="1">
+      <c r="F3" s="14"/>
+      <c r="G3" s="12">
         <v>5</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="12">
+        <v>200</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="12">
+        <v>5</v>
+      </c>
+      <c r="H4" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="I3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="20" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="12">
+        <v>5</v>
+      </c>
+      <c r="H5" s="12">
+        <v>2200</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="D6" s="12"/>
+      <c r="E6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="12">
         <v>5</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H6" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="L7" s="16"/>
+    </row>
+    <row r="8" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="12">
+        <v>5</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="16"/>
+    </row>
+    <row r="9" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="12">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="20" t="s">
+      <c r="H9" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="16"/>
+    </row>
+    <row r="10" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="D10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="12">
+        <v>10</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:14" s="17" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="12">
+        <v>10</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="12">
+        <v>20</v>
+      </c>
+      <c r="H12" s="12">
+        <v>800</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="12">
+        <v>20</v>
+      </c>
+      <c r="H13" s="12">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="12">
+        <v>25</v>
+      </c>
+      <c r="H14" s="12">
+        <v>800</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="12">
+        <v>20</v>
+      </c>
+      <c r="H15" s="12">
+        <v>800</v>
+      </c>
+      <c r="M15" s="17">
+        <v>25</v>
+      </c>
+      <c r="N15" s="17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="12">
+        <v>20</v>
+      </c>
+      <c r="H16" s="12">
+        <v>800</v>
+      </c>
+      <c r="I16" s="17">
+        <v>3</v>
+      </c>
+      <c r="K16" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="17" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="1">
-        <v>5</v>
-      </c>
-      <c r="H5" s="1">
-        <v>15</v>
-      </c>
-      <c r="J5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="20" t="s">
+      <c r="F17" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="12">
+        <v>25</v>
+      </c>
+      <c r="H17" s="12">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="17" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="1">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="20" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="12">
+        <v>20</v>
+      </c>
+      <c r="H18" s="12">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="17" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="1">
-        <v>5</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="20" t="s">
+      <c r="C19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" s="12">
+        <v>30</v>
+      </c>
+      <c r="H19" s="12">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="17" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G8" s="1">
-        <v>5</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="12">
+        <v>30</v>
+      </c>
+      <c r="H20" s="12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="17" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="12">
+        <v>30</v>
+      </c>
+      <c r="H21" s="12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="17" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="G22" s="12">
         <v>40</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="1">
-        <v>15</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="1">
-        <v>10</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="1">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G12" s="1">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1">
-        <v>25</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="1">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14" s="1">
-        <v>25</v>
-      </c>
-      <c r="H14" s="1">
-        <v>25</v>
-      </c>
-      <c r="M14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="1">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1">
-        <v>25</v>
-      </c>
-      <c r="M15">
-        <v>25</v>
-      </c>
-      <c r="N15">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G16" s="1">
-        <v>20</v>
-      </c>
-      <c r="H16" s="14">
-        <v>25</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="K16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="1">
-        <v>25</v>
-      </c>
-      <c r="H17" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="1">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="1">
-        <v>30</v>
-      </c>
-      <c r="H19" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" s="1">
-        <v>30</v>
-      </c>
-      <c r="H20" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="1">
-        <v>30</v>
-      </c>
-      <c r="H21" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="1">
-        <v>35</v>
-      </c>
-      <c r="H22" s="1"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="18"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>4</v>
       </c>
       <c r="I24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F29" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F30" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C31" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="H31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2105,7 +2079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B431F8E3-B7EE-47D3-9B94-7C96A4B130FE}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2120,25 +2094,25 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2208,7 +2182,7 @@
         <v>300</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F3:F6" si="0">D4/E4</f>
+        <f t="shared" ref="F4:F6" si="0">D4/E4</f>
         <v>9.3333333333333339</v>
       </c>
       <c r="G4" s="1">
@@ -2272,25 +2246,25 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s">
         <v>142</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>143</v>
-      </c>
-      <c r="D15" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="8">
         <v>0</v>
       </c>
     </row>
@@ -2298,7 +2272,7 @@
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17" s="25">
+      <c r="C17" s="8">
         <v>200</v>
       </c>
       <c r="D17">
@@ -2309,11 +2283,11 @@
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="8">
         <v>500</v>
       </c>
       <c r="D18">
-        <f>C18-C17</f>
+        <f t="shared" ref="D18:D23" si="1">C18-C17</f>
         <v>300</v>
       </c>
     </row>
@@ -2321,11 +2295,11 @@
       <c r="B19">
         <v>4</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="9">
         <v>900</v>
       </c>
       <c r="D19">
-        <f>C19-C18</f>
+        <f t="shared" si="1"/>
         <v>400</v>
       </c>
     </row>
@@ -2333,11 +2307,11 @@
       <c r="B20">
         <v>5</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="9">
         <v>1400</v>
       </c>
       <c r="D20">
-        <f>C20-C19</f>
+        <f t="shared" si="1"/>
         <v>500</v>
       </c>
     </row>
@@ -2345,11 +2319,11 @@
       <c r="B21">
         <v>6</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="9">
         <v>2000</v>
       </c>
       <c r="D21">
-        <f>C21-C20</f>
+        <f t="shared" si="1"/>
         <v>600</v>
       </c>
     </row>
@@ -2357,11 +2331,11 @@
       <c r="B22">
         <v>7</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="10">
         <v>2800</v>
       </c>
       <c r="D22">
-        <f>C22-C21</f>
+        <f t="shared" si="1"/>
         <v>800</v>
       </c>
     </row>
@@ -2369,11 +2343,11 @@
       <c r="B23">
         <v>8</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="10">
         <v>3800</v>
       </c>
       <c r="D23">
-        <f>C23-C22</f>
+        <f t="shared" si="1"/>
         <v>1000</v>
       </c>
     </row>
@@ -2381,11 +2355,11 @@
       <c r="B24">
         <v>9</v>
       </c>
-      <c r="C24" s="27">
+      <c r="C24" s="10">
         <v>5100</v>
       </c>
       <c r="D24">
-        <f t="shared" ref="D19:D35" si="1">C24-C23</f>
+        <f t="shared" ref="D24:D35" si="2">C24-C23</f>
         <v>1300</v>
       </c>
     </row>
@@ -2393,11 +2367,11 @@
       <c r="B25">
         <v>10</v>
       </c>
-      <c r="C25" s="24">
+      <c r="C25" s="7">
         <v>6700</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1600</v>
       </c>
     </row>
@@ -2405,11 +2379,11 @@
       <c r="B26">
         <v>11</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="7">
         <v>8700</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
     </row>
@@ -2417,11 +2391,11 @@
       <c r="B27">
         <v>12</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="7">
         <v>11100</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2400</v>
       </c>
     </row>
@@ -2429,11 +2403,11 @@
       <c r="B28">
         <v>13</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="7">
         <v>13900</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2800</v>
       </c>
     </row>
@@ -2441,11 +2415,11 @@
       <c r="B29">
         <v>14</v>
       </c>
-      <c r="C29" s="24">
+      <c r="C29" s="7">
         <v>17400</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3500</v>
       </c>
     </row>
@@ -2457,7 +2431,7 @@
         <v>21400</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4000</v>
       </c>
     </row>
@@ -2469,7 +2443,7 @@
         <v>25900</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4500</v>
       </c>
     </row>
@@ -2517,7 +2491,7 @@
         <v>62700</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10000</v>
       </c>
     </row>
@@ -2530,7 +2504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9076AE7E-FB59-4599-805D-C36A527D9B9A}">
   <dimension ref="B3:C39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2543,100 +2517,100 @@
   <sheetData>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>